<commit_message>
added Man O Arms Talents
</commit_message>
<xml_diff>
--- a/Talent Spreadsheet.xlsx
+++ b/Talent Spreadsheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="112">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -73,10 +73,10 @@
     <t xml:space="preserve">4,5</t>
   </si>
   <si>
-    <t xml:space="preserve">Ignore Pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You may now use 5+CON as you wound threshold</t>
+    <t xml:space="preserve">Toughness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While wearing Light or no armor, you may subtract your fortitude from any attacks made against you. This cannot stack with Guard Stance or other similar effects.</t>
   </si>
   <si>
     <t xml:space="preserve">5,6</t>
@@ -102,10 +102,10 @@
     <t xml:space="preserve">7,8,9</t>
   </si>
   <si>
-    <t xml:space="preserve">Toughness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While wearing Light or no armor, you may subtract your fortitude from any attacks made against you. This cannot stack with Guard Stance or other similar effects.</t>
+    <t xml:space="preserve">Ignore Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may now use 5+CON as you wound threshold</t>
   </si>
   <si>
     <t xml:space="preserve">Increadible Momentum</t>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t xml:space="preserve">10,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Man O’ Arms – 5: Heavy Strikes</t>
   </si>
   <si>
     <t xml:space="preserve">Fighting Combo</t>
@@ -222,6 +225,25 @@
     <t xml:space="preserve">9,10</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Man O’ Arms – 6: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Weapon Criticals</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Opportunist</t>
   </si>
   <si>
@@ -288,7 +310,7 @@
     <t xml:space="preserve">Perfect Posture</t>
   </si>
   <si>
-    <t xml:space="preserve">When using only one one handed or a versatile weapon with nothing in your off hand. Increase your Guard Defense by 5 and your to hit with that weapon by 5</t>
+    <t xml:space="preserve">When using only one one-handed or a versatile weapon, with no sheild in your off hand, increase your Guard Defense by 5 and your to hit with that weapon by 5</t>
   </si>
   <si>
     <t xml:space="preserve">Heavy Strikes</t>
@@ -310,9 +332,6 @@
 [Hammers and Blunt Polearms] 7 – Bone Break: Each successful melee attack made against the target after this effect is applied deals +2 damage. This effect can be removed that same way a bleeding or wounded effect can be removed.</t>
   </si>
   <si>
-    <t xml:space="preserve">9,10,11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Consecutive Strikes</t>
   </si>
   <si>
@@ -322,13 +341,103 @@
     <t xml:space="preserve">Sword and Board</t>
   </si>
   <si>
-    <t xml:space="preserve">Gain +10 to your roll when counter striking with a shield in one hand  and the weapon in the other.</t>
+    <t xml:space="preserve">Gain +10 to your roll when counter striking with a shield in one hand and the weapon in the other.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berserker – 6: Ignore Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,13,14,15,16</t>
   </si>
   <si>
     <t xml:space="preserve">Quick Draw</t>
   </si>
   <si>
     <t xml:space="preserve">You may now Stow weapons and Draw a new weapon as part of any attack action or aim action for range weapons. The proper holster spot for drawing and stowing must be easily available on your body.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Footwork Expertise</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Twice per short rest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, you may use this ability to ignore the penalty of using a polearm with reach at 5ft, or to give a polearm that does not have the reach property (including when holding in one hand) the reach property. Regardless of which effect is chosen, this will last until the next time you hit with an polearm attack.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lumberjack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Expertise</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Twice per short rest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, you may use this ability to cause your next hit with an Axe weapon to ignore armor (Deals 100% damage to the target and their armor). This must be used before the attack roll is made.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge Alignment Expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twice per short rest when performing an attack using the blade skill, you may use this ability to change the roll of your small d10 to 5. This affects both damage and to hit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forceful Striking Expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twice per short rest after performing an attack using the hammers skill, you may use this ability to deal the same damage to the targets armor again. This does not deal damage to the targets vitality. It is as if the armor took two  identical his from one attack.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shield Strike Expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twice per short rest while performing a successful shield bash attack, instead of the shields normal effect, you may give your target the stun 1 condition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weapons Expert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once per long rest. You may chose one of the previous expertise skills that you know, and reset its charges. This can be done at any time.</t>
   </si>
 </sst>
 </file>
@@ -338,11 +447,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -360,134 +470,20 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -495,23 +491,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -535,57 +516,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -609,91 +539,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -704,20 +557,23 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="62.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -733,14 +589,14 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -760,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -780,14 +636,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -800,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -820,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -840,14 +696,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -860,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -876,62 +732,65 @@
       <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G8" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>14</v>
@@ -940,58 +799,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>16</v>
@@ -1000,61 +859,61 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>10</v>
@@ -1079,22 +938,22 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="62.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1110,25 +969,25 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -1137,58 +996,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>8</v>
@@ -1202,53 +1061,56 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="68.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>10</v>
@@ -1257,21 +1119,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>5</v>
@@ -1282,16 +1144,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>5</v>
@@ -1302,16 +1164,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>5</v>
@@ -1322,13 +1184,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>15</v>
@@ -1342,13 +1204,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>15</v>
@@ -1357,18 +1219,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>16</v>
@@ -1377,18 +1239,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>16</v>
@@ -1397,41 +1259,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>10</v>
@@ -1453,10 +1315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1465,8 +1327,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="62.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -1487,7 +1349,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
@@ -1499,13 +1361,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -1519,16 +1381,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1</v>
@@ -1539,33 +1401,33 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>9</v>
@@ -1574,18 +1436,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>9</v>
@@ -1599,33 +1461,33 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>10</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>11</v>
@@ -1639,16 +1501,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
@@ -1659,30 +1524,36 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>5</v>
@@ -1693,60 +1564,138 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="B13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="G13" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="B14" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="G14" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="G15" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="B16" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="G16" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="B17" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="G17" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>